<commit_message>
임시 [AutoInput] 코드 작성
</commit_message>
<xml_diff>
--- a/document/DSF 시퀀스.xlsx
+++ b/document/DSF 시퀀스.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
   <si>
     <t>no</t>
   </si>
@@ -134,25 +134,25 @@
     <t>EventHostRackOutputConfirm</t>
   </si>
   <si>
-    <t>Rack 출고 완료 요청 with TrayId/RackId</t>
+    <t>Rack 출고 완료 보고 with TrayId/RackId</t>
   </si>
   <si>
     <t>EventEqpRackOutputCompleteRequest</t>
   </si>
   <si>
-    <t>Rack 출고 완료 요청 Confirm</t>
+    <t>Rack 출고 완료 보고 Confirm</t>
   </si>
   <si>
     <t>EventHostRackOutputCompleteConfirm</t>
   </si>
   <si>
-    <t>투입 Tray 투입 완료 요청</t>
+    <t>투입 Tray 투입 완료 보고</t>
   </si>
   <si>
     <t>EventEqpInletTrayInputCompleteRequest</t>
   </si>
   <si>
-    <t>투입 Tray 투입 완료 요청 Confirm</t>
+    <t>투입 Tray 투입 완료 보고 Confirm</t>
   </si>
   <si>
     <t>EventHostInletTrayInputCompleteConfirm</t>
@@ -200,13 +200,13 @@
     <t>EventHostTrayBreakCompleteConfirm</t>
   </si>
   <si>
-    <t>배출 Tray 투입 완료 요청</t>
+    <t>배출 Tray 투입 완료 보고</t>
   </si>
   <si>
     <t>EventEqpOutletTrayInputCompleteRequest</t>
   </si>
   <si>
-    <t>배출 Tray 투입 완료 요청 Confirm</t>
+    <t>배출 Tray 투입 완료 보고 Confirm</t>
   </si>
   <si>
     <t>EventHostOutletTrayInputCompleteConfirm</t>
@@ -239,31 +239,34 @@
     <t>EventHostNGTrayBreakConfirm</t>
   </si>
   <si>
-    <t>NG Tray Break 완료 with TrayId</t>
+    <t>NG Tray Break 완료 보고 with TrayId</t>
   </si>
   <si>
     <t>EventEqpNGTrayBreakCompleteRequest</t>
   </si>
   <si>
-    <t>NG Tray Break 완료 Confirm</t>
+    <t>NG Tray Break 완료 보고 Confirm</t>
   </si>
   <si>
     <t>EventHostNGTrayBreakCompleteConfirm</t>
   </si>
   <si>
-    <t>NG Tray 투입 완료 요청</t>
+    <t>NG Tray 투입 완료 보고</t>
   </si>
   <si>
     <t>EventEqpNGTrayInputCompleteRequest</t>
   </si>
   <si>
-    <t>NG Tray 투입 완료 요청 Confirm</t>
+    <t>NG Tray 투입 완료 보고 Confirm</t>
   </si>
   <si>
     <t>EventHostNGTrayInputCompleteConfirm</t>
   </si>
   <si>
-    <t>[분기1 - 자동 투입] 자동 셀 투입 요청 with CellID</t>
+    <t>35_1_1</t>
+  </si>
+  <si>
+    <t>[분기1 - 자동 투입] 자동 셀 투입 요청 with CellID &amp; TrayID</t>
   </si>
   <si>
     <t>EventEqpAutoCellInputRequest</t>
@@ -272,42 +275,63 @@
     <t>분기1 - 자동 투입</t>
   </si>
   <si>
+    <t>35_1_2</t>
+  </si>
+  <si>
     <t>[분기1 - 자동 투입] 자동 셀 투입 요청 Confirm</t>
   </si>
   <si>
     <t>EventHostAutoCellInputConfirm</t>
   </si>
   <si>
-    <t>[분기1 - 자동 투입] 투입셀 정보 검사 요청 with CellID</t>
+    <t>35_1_3</t>
+  </si>
+  <si>
+    <t>[분기1 - 자동 투입] 투입셀 정보 검사 요청 with CellID &amp; TrayID</t>
   </si>
   <si>
     <t>EventEqpInputCellInfoInspectionRequest</t>
   </si>
   <si>
+    <t>35_1_4</t>
+  </si>
+  <si>
     <t>[분기1 - 자동 투입] 투입셀 정보 검사 요청 Confirm</t>
   </si>
   <si>
     <t>EventHostInputCellInfoInspectionConfirm</t>
   </si>
   <si>
-    <t>[분기1 - 자동 투입] 셀 공정 시작 보고</t>
+    <t>35_1_5</t>
+  </si>
+  <si>
+    <t>[분기1 - 자동 투입] 셀 공정 시작 보고 with CellID</t>
   </si>
   <si>
     <t>EventEqpCellProcessStartReport</t>
   </si>
   <si>
+    <t>35_1_6</t>
+  </si>
+  <si>
     <t>[분기1 - 자동 투입] 셀 공정 시작 보고 Confirm</t>
   </si>
   <si>
     <t>EventHostCellProcessStartConfirm</t>
   </si>
   <si>
-    <t xml:space="preserve">[분기1 - 자동 투입] 자동 셀 투입 완료보고 </t>
+    <t>35_1_7</t>
+  </si>
+  <si>
+    <t>[분기1 - 자동 투입] 자동 셀 투입 완료보고 with CellID &amp; TrayID</t>
   </si>
   <si>
     <t>EventEqpAutoCellInputCompleteReport</t>
   </si>
   <si>
+    <t>35_1_8</t>
+  </si>
+  <si>
     <t>[분기1 - 자동 투입] 자동 셀 투입 완료보고 Confirm</t>
   </si>
   <si>
@@ -329,7 +353,7 @@
     <t>EventHostManualCellInputConfirm</t>
   </si>
   <si>
-    <t>[분기2 - 수동 투입] 투입셀 정보 검사 요청 with CellID</t>
+    <t>[분기2 - 수동 투입] 투입셀 정보 검사 요청 with CellID &amp; TrayID</t>
   </si>
   <si>
     <t>[분기2 - 수동 투입] 투입셀 정보 검사 요청 Confirm</t>
@@ -1680,8 +1704,8 @@
   <sheetPr/>
   <dimension ref="B3:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -2202,115 +2226,115 @@
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="3">
-        <v>35</v>
+      <c r="B38" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="3">
-        <v>36</v>
+      <c r="B39" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="3">
-        <v>37</v>
+      <c r="B40" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="3">
-        <v>38</v>
+      <c r="B41" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="3">
-        <v>39</v>
+      <c r="B42" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="3">
-        <v>40</v>
+      <c r="B43" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="9" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="3">
-        <v>41</v>
+      <c r="B44" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="9" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="3">
-        <v>42</v>
+      <c r="B45" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="3"/>
@@ -2321,13 +2345,13 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G46" s="3"/>
     </row>
@@ -2337,10 +2361,10 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="10" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="3"/>
@@ -2351,10 +2375,10 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="10" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="3"/>
@@ -2365,10 +2389,10 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="10" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="3"/>
@@ -2379,10 +2403,10 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="10" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="3"/>
@@ -2393,10 +2417,10 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="10" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="3"/>
@@ -2407,7 +2431,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="10" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>28</v>
@@ -2421,7 +2445,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="10" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>30</v>
@@ -2435,10 +2459,10 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="10" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="3"/>
@@ -2449,10 +2473,10 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="10" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="3"/>
@@ -2463,13 +2487,13 @@
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="14" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="G56" s="3"/>
     </row>
@@ -2479,10 +2503,10 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="14" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="3"/>
@@ -2493,10 +2517,10 @@
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="14" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="3"/>
@@ -2507,10 +2531,10 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="14" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="3"/>
@@ -2521,10 +2545,10 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="14" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="3"/>
@@ -2535,10 +2559,10 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="14" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="3"/>
@@ -2549,13 +2573,13 @@
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="16" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G62" s="15"/>
     </row>
@@ -2565,14 +2589,14 @@
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="16" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="15" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -2581,10 +2605,10 @@
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="16" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="15"/>
@@ -2595,10 +2619,10 @@
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="16" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="15"/>
@@ -2609,13 +2633,13 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="17" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="G66" s="3"/>
     </row>
@@ -2625,10 +2649,10 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="17" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="3"/>
@@ -2639,10 +2663,10 @@
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="17" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="3"/>
@@ -2653,10 +2677,10 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="17" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="3"/>
@@ -2667,10 +2691,10 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="17" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="3"/>
@@ -2681,10 +2705,10 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="17" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="3"/>
@@ -2695,10 +2719,10 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="17" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="3"/>
@@ -2709,10 +2733,10 @@
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="17" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="3"/>
@@ -2723,10 +2747,10 @@
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="17" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="3"/>
@@ -2737,10 +2761,10 @@
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="17" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="3"/>
@@ -2751,13 +2775,13 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="18" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="G76" s="3"/>
     </row>
@@ -2767,10 +2791,10 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="18" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="F77" s="12"/>
       <c r="G77" s="3"/>
@@ -2781,10 +2805,10 @@
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="18" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F78" s="12"/>
       <c r="G78" s="3"/>
@@ -2795,10 +2819,10 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="18" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="F79" s="13"/>
       <c r="G79" s="3"/>
@@ -2809,13 +2833,13 @@
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="19" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="G80" s="15"/>
     </row>
@@ -2825,10 +2849,10 @@
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="19" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="F81" s="12"/>
       <c r="G81" s="15"/>
@@ -2839,10 +2863,10 @@
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="19" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="F82" s="12"/>
       <c r="G82" s="15"/>
@@ -2853,10 +2877,10 @@
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="19" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="F83" s="12"/>
       <c r="G83" s="15"/>
@@ -2867,10 +2891,10 @@
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="19" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="F84" s="12"/>
       <c r="G84" s="15"/>
@@ -2881,10 +2905,10 @@
       </c>
       <c r="C85" s="15"/>
       <c r="D85" s="19" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="15"/>

</xml_diff>